<commit_message>
Updated short IR sensor data spreadsheet
Added the data obtained from the sensors currently attached to the
working robot.
</commit_message>
<xml_diff>
--- a/Resources/Short IR Sensor Data.xlsx
+++ b/Resources/Short IR Sensor Data.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Family\Google Drive\Robotics\Personal iNexus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Family\Google Drive\Robotics\iNexus Personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="7635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="7635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>White Surface</t>
   </si>
@@ -62,8 +63,53 @@
     <t>data</t>
   </si>
   <si>
+    <t>352-478: -0.0159x + 12.566</t>
+  </si>
+  <si>
+    <t>224-352: -0.0309x + 17.779</t>
+  </si>
+  <si>
+    <t>110-224: y = -0.0855x + 29.804</t>
+  </si>
+  <si>
+    <t>79-110: y = -0.2774x + 51.38</t>
+  </si>
+  <si>
+    <t>-0.1586x + 125.66</t>
+  </si>
+  <si>
+    <t>-0.3093x + 177.79</t>
+  </si>
+  <si>
+    <t>-0.855x + 298.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -2.7738x + 513.8</t>
+  </si>
+  <si>
+    <t>100 Sample Average</t>
+  </si>
+  <si>
+    <t>x is cm, y is raw</t>
+  </si>
+  <si>
+    <t>x is raw, y is cm</t>
+  </si>
+  <si>
+    <t>x is raw, y is mm</t>
+  </si>
+  <si>
+    <t>Piecewise function</t>
+  </si>
+  <si>
+    <t>Raw</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
     <r>
-      <t>y = 1982.5x</t>
+      <t>y = 19825x</t>
     </r>
     <r>
       <rPr>
@@ -76,51 +122,12 @@
       <t>-0.96</t>
     </r>
   </si>
-  <si>
-    <t>352-478: -0.0159x + 12.566</t>
-  </si>
-  <si>
-    <t>224-352: -0.0309x + 17.779</t>
-  </si>
-  <si>
-    <t>110-224: y = -0.0855x + 29.804</t>
-  </si>
-  <si>
-    <t>79-110: y = -0.2774x + 51.38</t>
-  </si>
-  <si>
-    <t>-0.1586x + 125.66</t>
-  </si>
-  <si>
-    <t>-0.3093x + 177.79</t>
-  </si>
-  <si>
-    <t>-0.855x + 298.04</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -2.7738x + 513.8</t>
-  </si>
-  <si>
-    <t>100 Sample Average</t>
-  </si>
-  <si>
-    <t>x is cm, y is raw</t>
-  </si>
-  <si>
-    <t>x is raw, y is cm</t>
-  </si>
-  <si>
-    <t>x is raw, y is mm</t>
-  </si>
-  <si>
-    <t>Piecewise function</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,13 +144,6 @@
     <font>
       <vertAlign val="superscript"/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF595959"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -196,17 +196,14 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -312,7 +309,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -354,38 +351,86 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$I$20:$I$29</c:f>
+              <c:f>Sheet1!$I$4:$I$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>478</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="17">
                   <c:v>106</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="18">
                   <c:v>102</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="19">
                   <c:v>99</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="20">
                   <c:v>96</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="21">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="22">
                   <c:v>86</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="23">
                   <c:v>83</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="24">
                   <c:v>82</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="25">
                   <c:v>79</c:v>
                 </c:pt>
               </c:numCache>
@@ -393,38 +438,86 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$20:$K$29</c:f>
+              <c:f>Sheet1!$K$4:$K$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>210</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="17">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="18">
                   <c:v>230</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="19">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="20">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="21">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="22">
                   <c:v>270</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="23">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="24">
                   <c:v>290</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="25">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -440,11 +533,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="165299136"/>
-        <c:axId val="165299696"/>
+        <c:axId val="110023232"/>
+        <c:axId val="110023792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="165299136"/>
+        <c:axId val="110023232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -501,12 +594,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165299696"/>
+        <c:crossAx val="110023792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="165299696"/>
+        <c:axId val="110023792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,7 +656,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="165299136"/>
+        <c:crossAx val="110023232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -912,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,38 +1021,38 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="6" t="s">
-        <v>21</v>
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="5"/>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
         <v>11</v>
@@ -1115,10 +1208,10 @@
         <v>250</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="I9" s="3">
         <v>250</v>
@@ -1144,11 +1237,11 @@
       <c r="D10" s="3">
         <v>224</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>17</v>
+      <c r="F10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="I10" s="3">
         <v>224</v>
@@ -1172,11 +1265,11 @@
       <c r="D11" s="3">
         <v>211</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>18</v>
+      <c r="F11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="I11" s="3">
         <v>211</v>
@@ -1200,11 +1293,11 @@
       <c r="D12" s="3">
         <v>197</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>19</v>
+      <c r="F12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="I12" s="3">
         <v>197</v>
@@ -1228,11 +1321,11 @@
       <c r="D13" s="3">
         <v>181</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>20</v>
+      <c r="F13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="I13" s="3">
         <v>181</v>
@@ -1280,7 +1373,7 @@
         <v>158</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I15" s="3">
         <v>158</v>
@@ -1304,8 +1397,8 @@
       <c r="D16" s="3">
         <v>146</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>12</v>
+      <c r="F16" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="I16" s="3">
         <v>146</v>
@@ -1615,4 +1708,219 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>535</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>460</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>405</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>355</v>
+      </c>
+      <c r="B5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>315</v>
+      </c>
+      <c r="B6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>285</v>
+      </c>
+      <c r="B7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>260</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>237</v>
+      </c>
+      <c r="B9">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>222</v>
+      </c>
+      <c r="B10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>210</v>
+      </c>
+      <c r="B11">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>200</v>
+      </c>
+      <c r="B12">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>190</v>
+      </c>
+      <c r="B13">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>180</v>
+      </c>
+      <c r="B14">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>170</v>
+      </c>
+      <c r="B15">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>160</v>
+      </c>
+      <c r="B16">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>157</v>
+      </c>
+      <c r="B17">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>150</v>
+      </c>
+      <c r="B18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>140</v>
+      </c>
+      <c r="B19">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>135</v>
+      </c>
+      <c r="B20">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>132</v>
+      </c>
+      <c r="B21">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>127</v>
+      </c>
+      <c r="B22">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>125</v>
+      </c>
+      <c r="B23">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>122</v>
+      </c>
+      <c r="B24">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>120</v>
+      </c>
+      <c r="B25">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>